<commit_message>
updated the EEPROM, I2C_connect, ESD protection IC and updated the images
</commit_message>
<xml_diff>
--- a/Hardware/BOM_PCB_directMessage_seedfusion.xlsx
+++ b/Hardware/BOM_PCB_directMessage_seedfusion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PCB_directMessage_latest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -220,15 +220,6 @@
     <t>https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_XFCN-M2010RS-02P_C520130.html</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>USBLC6-2P6</t>
-  </si>
-  <si>
-    <t>https://lcsc.com/product-detail/ESD-Protection-Devices_STMicroelectronics-USBLC6-2P6_C15999.html</t>
-  </si>
-  <si>
     <t>R17</t>
   </si>
   <si>
@@ -250,12 +241,6 @@
     <t>I2C_CONNECT</t>
   </si>
   <si>
-    <t>2185-104ZG0CYNR1</t>
-  </si>
-  <si>
-    <t>https://lcsc.com/product-detail/Female-Headers_Wcon-2185-104ZG0CYNR1_C721891.html</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -367,12 +352,6 @@
     <t>U11</t>
   </si>
   <si>
-    <t>M24256-DRDW8TP/K</t>
-  </si>
-  <si>
-    <t>https://lcsc.com/product-detail/EEPROM_STMicroelectronics-M24256-DRDW8TP-K_C2061704.html</t>
-  </si>
-  <si>
     <t>R14,R15</t>
   </si>
   <si>
@@ -403,35 +382,57 @@
     <t>DISPLAY</t>
   </si>
   <si>
-    <t>ZJY180SN009</t>
-  </si>
-  <si>
-    <t>https://www.smart-prototyping.com/1_8-inch-TFT-LCD-Bare-Display-ST7735-SPI-128-160?search=1.8%20inch%20TFT%20LCD</t>
+    <t>TPD1E10B06DPYR</t>
+  </si>
+  <si>
+    <t>ESD1,ESD2,ESD3</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/TVS_Texas-Instruments-TPD1E10B06DPYR_C48260.html</t>
+  </si>
+  <si>
+    <t>MF254RS-11-05-0743</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Female-Headers_XFCN-MF254RS-11-05-0743_C668121.html</t>
+  </si>
+  <si>
+    <t>ZD24C128A-SSGMB</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/EEPROM_Zetta-ZD24C128A-SSGMB_C918271.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/3256803581858691.html?src=ibdm_d03p0558e02r02&amp;sk=&amp;aff_platform=&amp;aff_trace_key=&amp;af=&amp;cv=&amp;cn=&amp;dp=&amp;gatewayAdapt=4itemAdapt</t>
+  </si>
+  <si>
+    <t>Module ST7735</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -450,127 +451,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,192 +465,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -772,245 +478,46 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1299,24 +806,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.90909090909091" customWidth="1"/>
-    <col min="2" max="2" width="17.1090909090909" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="5" max="5" width="18.7727272727273" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1336,7 +843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.5" spans="1:5">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1353,7 +860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="14.5" spans="1:5">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1370,7 +877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="14.5" spans="1:5">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1387,7 +894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" ht="14.5" spans="1:5">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1404,7 +911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" ht="14.5" spans="1:5">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1421,7 +928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" ht="14.5" spans="1:5">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1438,7 +945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" ht="14.5" spans="1:5">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1455,7 +962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" ht="14.5" spans="1:5">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1472,7 +979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" ht="14.5" spans="1:5">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1489,7 +996,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" ht="14.5" spans="1:5">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1506,7 +1013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" ht="14.5" spans="1:5">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1523,7 +1030,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" ht="14.5" spans="1:5">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1540,7 +1047,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" ht="14.5" spans="1:5">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1557,7 +1064,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" ht="14.5" spans="1:5">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1574,7 +1081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" ht="14.5" spans="1:5">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1591,7 +1098,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" ht="14.5" spans="1:5">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1608,7 +1115,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" ht="14.5" spans="1:5">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1625,7 +1132,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" ht="14.5" spans="1:5">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1642,7 +1149,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" ht="14.5" spans="1:5">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1659,7 +1166,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" ht="14.5" spans="1:5">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1676,7 +1183,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" ht="14.5" spans="1:5">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1693,376 +1200,376 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" ht="14.5" spans="1:5">
-      <c r="A23" s="2">
+    <row r="23" spans="1:5" s="7" customFormat="1">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" ht="14.5" spans="1:5">
+      <c r="B23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="8">
+        <v>3</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" ht="14.5" spans="1:5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="7" customFormat="1">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" ht="14.5" spans="1:5">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" ht="14.5" spans="1:5">
+      <c r="C26" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" ht="14.5" spans="1:5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D28" s="2">
         <v>4</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" ht="14.5" spans="1:5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" ht="14.5" spans="1:5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" ht="14.5" spans="1:5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" ht="14.5" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" ht="14.5" spans="1:5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D33" s="2">
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" ht="14.5" spans="1:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" ht="14.5" spans="1:5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" ht="14.5" spans="1:5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D36" s="2">
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" ht="14.5" spans="1:5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D37" s="2">
         <v>1</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" ht="14.5" spans="1:5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D38" s="2">
         <v>1</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" ht="14.5" spans="1:5">
-      <c r="A39" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="7" customFormat="1">
+      <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" ht="14.5" spans="1:5">
+      <c r="B39" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D40" s="2">
         <v>2</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" ht="14.5" spans="1:5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D41" s="2">
         <v>18</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" ht="14.5" spans="1:5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" ht="14.5" spans="1:5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:5">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:5">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:5">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:5">
       <c r="A48" s="2"/>
     </row>
     <row r="49" spans="1:1">
@@ -2175,51 +1682,47 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://lcsc.com/product-detail/USB-Connectors_CIKI-TYPE-C-2-0-16PIN-SMT-3-OR_C2987387.html"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_XINGLIGHT-XL-1608SURC-06_C965799.html"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_XINGLIGHT-XL-1608UBC-04_C965807.html"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://lcsc.com/product-detail/RF-Connectors-Coaxial-Connectors_HJ-Tech-HJ-SMA362_C2905338.html"/>
-    <hyperlink ref="E7" r:id="rId5" display="https://lcsc.com/product-detail/Micro-Motor-Motor_KOTL-Z3OC1T8219731_C2894731.html"/>
-    <hyperlink ref="E8" r:id="rId6" display="https://lcsc.com/product-detail/Slide-Switches_Nidec-CL-SB-22B-12T_C2921665.html"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://lcsc.com/product-detail/Female-Headers_Wcon-2185-204ZS0CYNR2_C721893.html"/>
-    <hyperlink ref="E10" r:id="rId8" display="https://lcsc.com/product-detail/Satellite-Positioning-Modules_Quectel-L80-M39_C133488.html"/>
-    <hyperlink ref="E11" r:id="rId9" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Walsin-Tech-Corp-0603X106M6R3CT_C123608.html"/>
-    <hyperlink ref="E12" r:id="rId10" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3RBD4701V_C191778.html"/>
-    <hyperlink ref="E13" r:id="rId11" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3EKF1003V_C189597.html"/>
-    <hyperlink ref="E14" r:id="rId12" display="https://lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_Diodes-Incorporated-AP2112K-1-8TRG1_C176944.html"/>
-    <hyperlink ref="E15" r:id="rId13" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_FH-Guangdong-Fenghua-Advanced-Tech-0603F475M100NT_C108344.html"/>
-    <hyperlink ref="E16" r:id="rId14" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_XINGLIGHT-XL-1608SYGC-06_C965805.html"/>
-    <hyperlink ref="E17" r:id="rId15" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJPA3J471V_C441888.html"/>
-    <hyperlink ref="E18" r:id="rId16" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3EKF2001V_C192167.html"/>
-    <hyperlink ref="E19" r:id="rId17" display="https://lcsc.com/product-detail/Battery-Management-ICs_Microchip-Tech-MCP73831T-2ACI-OT_C424093.html"/>
-    <hyperlink ref="E20" r:id="rId18" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Murata-Electronics-GCM188R71H104KA57D_C85864.html"/>
-    <hyperlink ref="E21" r:id="rId19" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_PSA-Prosperity-Dielectrics-FN18X104K500PBG_C235731.html"/>
-    <hyperlink ref="E22" r:id="rId20" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_XFCN-M2010RS-02P_C520130.html"/>
-    <hyperlink ref="E23" r:id="rId21" display="https://lcsc.com/product-detail/ESD-Protection-Devices_STMicroelectronics-USBLC6-2P6_C15999.html"/>
-    <hyperlink ref="E24" r:id="rId22" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3EKF1001V_C118155.html"/>
-    <hyperlink ref="E25" r:id="rId23" display="https://lcsc.com/product-detail/DIP-Switches_Korean-Hroparts-Elec-EP-02KS_C2911510.html"/>
-    <hyperlink ref="E26" r:id="rId24" display="https://lcsc.com/product-detail/Female-Headers_Wcon-2185-104ZG0CYNR1_C721891.html"/>
-    <hyperlink ref="E27" r:id="rId25" display="https://lcsc.com/product-detail/USB-ICs_SILICON-LABS-CP2102N-A02-GQFN24R_C969151.html"/>
-    <hyperlink ref="E28" r:id="rId26" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_KEMET-C0603C104J5RAC_C490602.html"/>
-    <hyperlink ref="E30" r:id="rId27" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Murata-Electronics-GCM188R71E474KA64D_C161219.html"/>
-    <hyperlink ref="E31" r:id="rId28" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Murata-Electronics-GRM188R61E105KA12D_C77046.html"/>
-    <hyperlink ref="E32" r:id="rId29" display="https://lcsc.com/product-detail/Schottky-Barrier-Diodes-SBD_STMicroelectronics-BAT20JFILM_C155590.html"/>
-    <hyperlink ref="E33" r:id="rId30" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3GEYJ103V_C169849.html"/>
-    <hyperlink ref="E34" r:id="rId31" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJUP3D47R0V_C491217.html"/>
-    <hyperlink ref="E35" r:id="rId32" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_RALEC-RTT03R010FTP_C158899.html"/>
-    <hyperlink ref="E36" r:id="rId33" display="https://lcsc.com/product-detail/Humidity-Sensors-Temperature-and-Humidity-Sensors_Bosch-Sensortec-BME280_C92489.html"/>
-    <hyperlink ref="E37" r:id="rId34" display="https://lcsc.com/product-detail/Battery-Management-ICs_Texas-Instruments-BQ27441DRZR-G1A_C473397.html"/>
-    <hyperlink ref="E38" r:id="rId35" display="https://lcsc.com/product-detail/MOSFETs_KUU-BSS138_C3015220.html"/>
-    <hyperlink ref="E39" r:id="rId36" display="https://lcsc.com/product-detail/EEPROM_STMicroelectronics-M24256-DRDW8TP-K_C2061704.html"/>
-    <hyperlink ref="E40" r:id="rId37" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3RBD5101V_C191782.html"/>
-    <hyperlink ref="E41" r:id="rId38" display="https://lcsc.com/product-detail/Tactile-Switches_ALPSALPINE-SKRPABE010_C115360.html"/>
-    <hyperlink ref="E42" r:id="rId39" display="https://lcsc.com/product-detail/Attitude-Sensors_TDK-InvenSense-MPU-9250_C71459.html"/>
-    <hyperlink ref="E6" r:id="rId40" display="https://www.seeedstudio.com/lora-e5-wireless-module-p-4745.html?queryID=adbf8c8b535a49e8361d053e0295bd14&amp;objectID=4745&amp;indexName=bazaar_retailer_products"/>
-    <hyperlink ref="E43" r:id="rId41" display="https://www.smart-prototyping.com/1_8-inch-TFT-LCD-Bare-Display-ST7735-SPI-128-160?search=1.8%20inch%20TFT%20LCD"/>
-    <hyperlink ref="E29" r:id="rId42" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC---SMD-SMT_CCTC-TCC0603X7R103M500CT_C376807.html"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E10" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="E15" r:id="rId13"/>
+    <hyperlink ref="E16" r:id="rId14"/>
+    <hyperlink ref="E17" r:id="rId15"/>
+    <hyperlink ref="E18" r:id="rId16"/>
+    <hyperlink ref="E19" r:id="rId17"/>
+    <hyperlink ref="E20" r:id="rId18"/>
+    <hyperlink ref="E21" r:id="rId19"/>
+    <hyperlink ref="E22" r:id="rId20"/>
+    <hyperlink ref="E24" r:id="rId21"/>
+    <hyperlink ref="E25" r:id="rId22"/>
+    <hyperlink ref="E27" r:id="rId23"/>
+    <hyperlink ref="E28" r:id="rId24"/>
+    <hyperlink ref="E30" r:id="rId25"/>
+    <hyperlink ref="E31" r:id="rId26"/>
+    <hyperlink ref="E32" r:id="rId27"/>
+    <hyperlink ref="E33" r:id="rId28"/>
+    <hyperlink ref="E34" r:id="rId29"/>
+    <hyperlink ref="E35" r:id="rId30"/>
+    <hyperlink ref="E36" r:id="rId31"/>
+    <hyperlink ref="E37" r:id="rId32"/>
+    <hyperlink ref="E38" r:id="rId33"/>
+    <hyperlink ref="E40" r:id="rId34"/>
+    <hyperlink ref="E41" r:id="rId35"/>
+    <hyperlink ref="E42" r:id="rId36"/>
+    <hyperlink ref="E6" r:id="rId37"/>
+    <hyperlink ref="E43" r:id="rId38"/>
+    <hyperlink ref="E29" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the readme file with the hardware features
</commit_message>
<xml_diff>
--- a/Hardware/BOM_PCB_directMessage_seedfusion.xlsx
+++ b/Hardware/BOM_PCB_directMessage_seedfusion.xlsx
@@ -403,10 +403,10 @@
     <t>https://lcsc.com/product-detail/EEPROM_Zetta-ZD24C128A-SSGMB_C918271.html</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/3256803581858691.html?src=ibdm_d03p0558e02r02&amp;sk=&amp;aff_platform=&amp;aff_trace_key=&amp;af=&amp;cv=&amp;cn=&amp;dp=&amp;gatewayAdapt=4itemAdapt</t>
-  </si>
-  <si>
     <t>Module ST7735</t>
+  </si>
+  <si>
+    <t>https://www.smart-prototyping.com/1_8-inch-TFT-LCD-Bare-Display-ST7735-SPI-128-160?search=1.8%20inch%20TFT%20LCD</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
   <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1548,13 +1548,13 @@
         <v>121</v>
       </c>
       <c r="C43" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:5">

</xml_diff>